<commit_message>
end of season round up
</commit_message>
<xml_diff>
--- a/data/DL24-25.xlsx
+++ b/data/DL24-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0001c2a442dfed87/Documents/Dream/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3531" documentId="8_{4A520963-05AC-46D2-973E-A3A248908BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{210327AB-77DA-4608-A383-1B4F73839A24}"/>
+  <xr:revisionPtr revIDLastSave="3844" documentId="8_{4A520963-05AC-46D2-973E-A3A248908BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F581E6B-1B75-4328-918D-747FD2CCD9C6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="366">
   <si>
     <t>TONY APPLETON</t>
   </si>
@@ -1112,6 +1112,27 @@
   </si>
   <si>
     <t>OISIN McENTEE</t>
+  </si>
+  <si>
+    <t>MARCO ASENSIO</t>
+  </si>
+  <si>
+    <t>1 (1-0)</t>
+  </si>
+  <si>
+    <t>2 (3-1)</t>
+  </si>
+  <si>
+    <t>ALISSON BECKER</t>
+  </si>
+  <si>
+    <t>MALIK MOTHERSILLE</t>
+  </si>
+  <si>
+    <t>-1 (0-1)</t>
+  </si>
+  <si>
+    <t>1 (2-1)</t>
   </si>
 </sst>
 </file>
@@ -1534,9 +1555,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1569,6 +1587,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1950,9 +1971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M351"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.9" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1963,7 +1982,7 @@
     <col min="5" max="5" width="10.6640625" style="44" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" style="68" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="67" customWidth="1"/>
     <col min="9" max="9" width="23.77734375" style="19" customWidth="1"/>
     <col min="10" max="10" width="31.44140625" style="19" customWidth="1"/>
     <col min="11" max="12" width="12" style="19" customWidth="1"/>
@@ -1979,7 +1998,7 @@
       <c r="E1" s="16"/>
       <c r="F1" s="15"/>
       <c r="G1" s="17"/>
-      <c r="H1" s="64"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="15" t="s">
@@ -1991,7 +2010,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="15"/>
       <c r="G2" s="17"/>
-      <c r="H2" s="70" t="s">
+      <c r="H2" s="69" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2001,7 +2020,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="15"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="64"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:13" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
@@ -2020,7 +2039,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="17"/>
-      <c r="H4" s="64"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="21" t="s">
         <v>6</v>
       </c>
@@ -2051,11 +2070,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="29">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G5" s="50"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="69" t="str">
+      <c r="H5" s="63"/>
+      <c r="I5" s="68" t="str">
         <f>D2</f>
         <v>TONY APPLETON</v>
       </c>
@@ -2065,15 +2084,15 @@
       </c>
       <c r="K5" s="30">
         <f t="shared" ref="K5:K17" si="0">L5-M5</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="L5" s="31">
         <f>SUM(F8:F25)</f>
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="M5" s="32">
         <f>SUM(F5:F7)</f>
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2083,7 +2102,7 @@
       <c r="E6" s="28"/>
       <c r="F6" s="27"/>
       <c r="G6" s="50"/>
-      <c r="H6" s="65"/>
+      <c r="H6" s="64"/>
       <c r="I6" s="15" t="str">
         <f>D29</f>
         <v>IAN RADCLIFFE</v>
@@ -2094,15 +2113,15 @@
       </c>
       <c r="K6" s="30">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L6" s="31">
         <f>SUM(F35:F52)</f>
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="M6" s="32">
         <f>SUM(F32:F34)</f>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2112,7 +2131,7 @@
       <c r="E7" s="28"/>
       <c r="F7" s="27"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="66"/>
+      <c r="H7" s="65"/>
       <c r="I7" s="15" t="str">
         <f>D56</f>
         <v>ROBIN MARSHALL</v>
@@ -2123,15 +2142,15 @@
       </c>
       <c r="K7" s="30">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="L7" s="31">
         <f>SUM(F62:F79)</f>
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="M7" s="32">
         <f>SUM(F59:F61)</f>
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2150,7 +2169,7 @@
       <c r="F8" s="33">
         <v>1</v>
       </c>
-      <c r="H8" s="65"/>
+      <c r="H8" s="64"/>
       <c r="I8" s="15" t="str">
         <f>D83</f>
         <v>TED LINEHAN</v>
@@ -2161,15 +2180,15 @@
       </c>
       <c r="K8" s="30">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="L8" s="31">
         <f>SUM(F89:F106)</f>
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M8" s="32">
         <f>SUM(F86:F88)</f>
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2186,9 +2205,9 @@
         <v>1</v>
       </c>
       <c r="F9" s="33">
-        <v>1</v>
-      </c>
-      <c r="H9" s="65"/>
+        <v>2</v>
+      </c>
+      <c r="H9" s="64"/>
       <c r="I9" s="15" t="str">
         <f>D110</f>
         <v>MARK TYLDESLEY</v>
@@ -2199,15 +2218,15 @@
       </c>
       <c r="K9" s="30">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L9" s="31">
         <f>SUM(F116:F133)</f>
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="M9" s="32">
         <f>SUM(F113:F115)</f>
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2224,9 +2243,9 @@
         <v>1</v>
       </c>
       <c r="F10" s="33">
-        <v>5</v>
-      </c>
-      <c r="H10" s="65"/>
+        <v>6</v>
+      </c>
+      <c r="H10" s="64"/>
       <c r="I10" s="15" t="str">
         <f>D137</f>
         <v>ANDY PETERSON</v>
@@ -2237,34 +2256,37 @@
       </c>
       <c r="K10" s="30">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="L10" s="31">
         <f>SUM(F143:F160)</f>
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="M10" s="32">
         <f>SUM(F140:F142)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="34">
-        <v>1</v>
-      </c>
-      <c r="F11" s="33">
+      <c r="E11" s="60">
+        <v>1</v>
+      </c>
+      <c r="F11" s="46">
         <v>8</v>
       </c>
-      <c r="H11" s="65"/>
+      <c r="G11" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="64"/>
       <c r="I11" s="15" t="str">
         <f>D164</f>
         <v>BRYN COOMBE</v>
@@ -2275,38 +2297,37 @@
       </c>
       <c r="K11" s="30">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L11" s="31">
         <f>SUM(F170:F187)</f>
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="M11" s="32">
         <f>SUM(F167:F169)</f>
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="61">
-        <v>1</v>
-      </c>
-      <c r="F12" s="46">
+      <c r="C12" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F12" s="33">
         <v>3</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="H12" s="65"/>
-      <c r="I12" s="15" t="str">
+      <c r="H12" s="66">
+        <v>45721</v>
+      </c>
+      <c r="I12" s="35" t="str">
         <f>D191</f>
         <v>GARY COOMBE</v>
       </c>
@@ -2316,37 +2337,37 @@
       </c>
       <c r="K12" s="30">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L12" s="31">
         <f>SUM(F197:F214)</f>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M12" s="32">
         <f>SUM(F194:F196)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="D13" s="33" t="s">
+      <c r="C13" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="F13" s="33">
-        <v>0</v>
-      </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="67">
-        <v>45704</v>
-      </c>
+      <c r="E13" s="60">
+        <v>1</v>
+      </c>
+      <c r="F13" s="46">
+        <v>3</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="66"/>
       <c r="I13" s="35" t="str">
         <f>D218</f>
         <v>GARETH HOSFORD</v>
@@ -2357,24 +2378,37 @@
       </c>
       <c r="K13" s="30">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L13" s="31">
         <f>SUM(F224:F241)</f>
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="M13" s="32">
         <f>SUM(F221:F223)</f>
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="53"/>
-      <c r="H14" s="67"/>
+      <c r="B14" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="33">
+        <v>3</v>
+      </c>
+      <c r="G14" s="45"/>
+      <c r="H14" s="66">
+        <v>45704</v>
+      </c>
       <c r="I14" s="35" t="str">
         <f>+D245</f>
         <v>JULIAN SLADE</v>
@@ -2389,11 +2423,11 @@
       </c>
       <c r="L14" s="31">
         <f>SUM(F251:F268)</f>
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="M14" s="32">
         <f>SUM(F248:F250)</f>
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2410,10 +2444,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="33">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G15" s="45"/>
-      <c r="H15" s="66"/>
+      <c r="H15" s="65"/>
       <c r="I15" s="35" t="str">
         <f>+D272</f>
         <v>CONAL HENRY</v>
@@ -2424,15 +2458,15 @@
       </c>
       <c r="K15" s="30">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L15" s="31">
         <f>SUM(F277:F295)</f>
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="M15" s="32">
         <f>SUM(F275:F276)</f>
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2445,7 +2479,7 @@
       <c r="D16" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="E16" s="61">
+      <c r="E16" s="60">
         <v>1</v>
       </c>
       <c r="F16" s="46">
@@ -2454,7 +2488,7 @@
       <c r="G16" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H16" s="64"/>
+      <c r="H16" s="63"/>
       <c r="I16" s="35" t="str">
         <f>+D299</f>
         <v>GORDON PETERSON</v>
@@ -2465,15 +2499,15 @@
       </c>
       <c r="K16" s="30">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L16" s="31">
         <f>SUM(F305:F322)</f>
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="M16" s="32">
         <f>SUM(F302:F304)</f>
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -2486,7 +2520,7 @@
       <c r="D17" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F17" s="46">
@@ -2495,7 +2529,7 @@
       <c r="G17" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H17" s="67">
+      <c r="H17" s="66">
         <v>45551</v>
       </c>
       <c r="I17" s="35" t="str">
@@ -2507,15 +2541,15 @@
       </c>
       <c r="K17" s="30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L17" s="31">
         <f>SUM(F332:F349)</f>
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="M17" s="32">
         <f>SUM(F329:F331)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2532,9 +2566,9 @@
         <v>253</v>
       </c>
       <c r="F18" s="33">
-        <v>1</v>
-      </c>
-      <c r="H18" s="67">
+        <v>2</v>
+      </c>
+      <c r="H18" s="66">
         <v>45693</v>
       </c>
       <c r="I18" s="36"/>
@@ -2553,7 +2587,7 @@
       <c r="D19" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="E19" s="61">
+      <c r="E19" s="60">
         <v>1</v>
       </c>
       <c r="F19" s="46">
@@ -2562,7 +2596,7 @@
       <c r="G19" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H19" s="64"/>
+      <c r="H19" s="63"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
@@ -2584,7 +2618,7 @@
         <v>14</v>
       </c>
       <c r="G20" s="45"/>
-      <c r="H20" s="67">
+      <c r="H20" s="66">
         <v>45515</v>
       </c>
     </row>
@@ -2598,7 +2632,7 @@
       <c r="D21" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="61">
+      <c r="E21" s="60">
         <v>1</v>
       </c>
       <c r="F21" s="46">
@@ -2607,7 +2641,7 @@
       <c r="G21" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H21" s="64"/>
+      <c r="H21" s="63"/>
     </row>
     <row r="22" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="46" t="s">
@@ -2626,7 +2660,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="45"/>
-      <c r="H22" s="67">
+      <c r="H22" s="66">
         <v>45515</v>
       </c>
     </row>
@@ -2640,7 +2674,7 @@
       <c r="D23" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="E23" s="61">
+      <c r="E23" s="60">
         <v>1</v>
       </c>
       <c r="F23" s="46">
@@ -2649,7 +2683,7 @@
       <c r="G23" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H23" s="67"/>
+      <c r="H23" s="66"/>
     </row>
     <row r="24" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
@@ -2661,14 +2695,14 @@
       <c r="D24" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F24" s="46">
         <v>2</v>
       </c>
       <c r="G24" s="45"/>
-      <c r="H24" s="67">
+      <c r="H24" s="66">
         <v>45537</v>
       </c>
     </row>
@@ -2686,10 +2720,10 @@
         <v>253</v>
       </c>
       <c r="F25" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25" s="50"/>
-      <c r="H25" s="67">
+      <c r="H25" s="66">
         <v>45693</v>
       </c>
     </row>
@@ -2702,10 +2736,10 @@
       </c>
       <c r="F26" s="43">
         <f>SUM(F8:F25)-SUM(F5:F7)</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="64"/>
+      <c r="H26" s="63"/>
     </row>
     <row r="27" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="15"/>
@@ -2713,7 +2747,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="15"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="64"/>
+      <c r="H27" s="63"/>
     </row>
     <row r="28" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="15"/>
@@ -2721,7 +2755,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="15"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="64"/>
+      <c r="H28" s="63"/>
     </row>
     <row r="29" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="15" t="s">
@@ -2733,7 +2767,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="15"/>
       <c r="G29" s="17"/>
-      <c r="H29" s="64"/>
+      <c r="H29" s="63"/>
     </row>
     <row r="30" spans="2:13" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="15"/>
@@ -2741,7 +2775,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="15"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="64"/>
+      <c r="H30" s="63"/>
     </row>
     <row r="31" spans="2:13" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="20" t="s">
@@ -2760,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="64"/>
+      <c r="H31" s="63"/>
     </row>
     <row r="32" spans="2:13" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="26" t="s">
@@ -2772,46 +2806,58 @@
       <c r="D32" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="62">
+      <c r="E32" s="61">
         <v>6</v>
       </c>
-      <c r="F32" s="63">
+      <c r="F32" s="62">
         <v>8</v>
       </c>
       <c r="G32" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H32" s="64"/>
+      <c r="H32" s="63"/>
     </row>
     <row r="33" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="49" t="s">
         <v>294</v>
       </c>
-      <c r="E33" s="28" t="s">
-        <v>253</v>
-      </c>
-      <c r="F33" s="27">
-        <v>33</v>
+      <c r="E33" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" s="49">
+        <v>36</v>
       </c>
       <c r="G33" s="50"/>
-      <c r="H33" s="67">
+      <c r="H33" s="66">
         <v>45555</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="49"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="27"/>
+      <c r="B34" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="F34" s="27">
+        <v>3</v>
+      </c>
       <c r="G34" s="50"/>
-      <c r="H34" s="64"/>
+      <c r="H34" s="66">
+        <v>45734</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="46" t="s">
@@ -2830,7 +2876,7 @@
         <v>5</v>
       </c>
       <c r="G35" s="45"/>
-      <c r="H35" s="64"/>
+      <c r="H35" s="63"/>
     </row>
     <row r="36" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
@@ -2846,9 +2892,9 @@
         <v>12</v>
       </c>
       <c r="F36" s="33">
-        <v>14</v>
-      </c>
-      <c r="H36" s="64"/>
+        <v>15</v>
+      </c>
+      <c r="H36" s="63"/>
     </row>
     <row r="37" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="46" t="s">
@@ -2866,7 +2912,7 @@
       <c r="F37" s="33">
         <v>16</v>
       </c>
-      <c r="H37" s="64"/>
+      <c r="H37" s="63"/>
     </row>
     <row r="38" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="46" t="s">
@@ -2885,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="45"/>
-      <c r="H38" s="64"/>
+      <c r="H38" s="63"/>
     </row>
     <row r="39" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="46" t="s">
@@ -2897,7 +2943,7 @@
       <c r="D39" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="61">
+      <c r="E39" s="60">
         <v>4</v>
       </c>
       <c r="F39" s="46">
@@ -2906,7 +2952,7 @@
       <c r="G39" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H39" s="64"/>
+      <c r="H39" s="63"/>
     </row>
     <row r="40" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="46" t="s">
@@ -2918,7 +2964,7 @@
       <c r="D40" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="E40" s="61" t="s">
+      <c r="E40" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F40" s="46">
@@ -2927,7 +2973,7 @@
       <c r="G40" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H40" s="67">
+      <c r="H40" s="66">
         <v>45523</v>
       </c>
     </row>
@@ -2945,9 +2991,9 @@
         <v>253</v>
       </c>
       <c r="F41" s="33">
-        <v>5</v>
-      </c>
-      <c r="H41" s="67">
+        <v>10</v>
+      </c>
+      <c r="H41" s="66">
         <v>45642</v>
       </c>
     </row>
@@ -2965,10 +3011,10 @@
         <v>23</v>
       </c>
       <c r="F42" s="33">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G42" s="45"/>
-      <c r="H42" s="64"/>
+      <c r="H42" s="63"/>
     </row>
     <row r="43" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="46" t="s">
@@ -2980,7 +3026,7 @@
       <c r="D43" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="61">
+      <c r="E43" s="60">
         <v>10</v>
       </c>
       <c r="F43" s="46">
@@ -2989,7 +3035,7 @@
       <c r="G43" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H43" s="64"/>
+      <c r="H43" s="63"/>
     </row>
     <row r="44" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="46" t="s">
@@ -3007,7 +3053,7 @@
       <c r="F44" s="33">
         <v>8</v>
       </c>
-      <c r="H44" s="67">
+      <c r="H44" s="66">
         <v>45621</v>
       </c>
     </row>
@@ -3021,7 +3067,7 @@
       <c r="D45" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="E45" s="61">
+      <c r="E45" s="60">
         <v>1</v>
       </c>
       <c r="F45" s="46">
@@ -3030,7 +3076,7 @@
       <c r="G45" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H45" s="64"/>
+      <c r="H45" s="63"/>
     </row>
     <row r="46" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="46" t="s">
@@ -3042,7 +3088,7 @@
       <c r="D46" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="E46" s="61" t="s">
+      <c r="E46" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F46" s="46">
@@ -3051,7 +3097,7 @@
       <c r="G46" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H46" s="67">
+      <c r="H46" s="66">
         <v>45523</v>
       </c>
     </row>
@@ -3069,9 +3115,9 @@
         <v>253</v>
       </c>
       <c r="F47" s="33">
-        <v>14</v>
-      </c>
-      <c r="H47" s="67">
+        <v>15</v>
+      </c>
+      <c r="H47" s="66">
         <v>45578</v>
       </c>
     </row>
@@ -3085,7 +3131,7 @@
       <c r="D48" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="E48" s="61">
+      <c r="E48" s="60">
         <v>4</v>
       </c>
       <c r="F48" s="46">
@@ -3094,7 +3140,7 @@
       <c r="G48" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H48" s="67"/>
+      <c r="H48" s="66"/>
     </row>
     <row r="49" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="46" t="s">
@@ -3106,7 +3152,7 @@
       <c r="D49" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="E49" s="61" t="s">
+      <c r="E49" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F49" s="46">
@@ -3115,7 +3161,7 @@
       <c r="G49" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H49" s="67">
+      <c r="H49" s="66">
         <v>45531</v>
       </c>
     </row>
@@ -3135,7 +3181,7 @@
       <c r="F50" s="33">
         <v>12</v>
       </c>
-      <c r="H50" s="67">
+      <c r="H50" s="66">
         <v>45565</v>
       </c>
     </row>
@@ -3149,7 +3195,7 @@
       <c r="D51" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="61">
+      <c r="E51" s="60">
         <v>1</v>
       </c>
       <c r="F51" s="46">
@@ -3158,7 +3204,7 @@
       <c r="G51" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H51" s="67"/>
+      <c r="H51" s="66"/>
     </row>
     <row r="52" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="48" t="s">
@@ -3174,10 +3220,10 @@
         <v>253</v>
       </c>
       <c r="F52" s="29">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G52" s="17"/>
-      <c r="H52" s="67">
+      <c r="H52" s="66">
         <v>45543</v>
       </c>
     </row>
@@ -3190,7 +3236,7 @@
       </c>
       <c r="F53" s="43">
         <f>SUM(F35:F52)-SUM(F32:F34)</f>
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G53" s="17"/>
     </row>
@@ -3200,7 +3246,7 @@
       <c r="E54" s="16"/>
       <c r="F54" s="15"/>
       <c r="G54" s="17"/>
-      <c r="H54" s="64"/>
+      <c r="H54" s="63"/>
     </row>
     <row r="55" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="15"/>
@@ -3208,7 +3254,7 @@
       <c r="E55" s="16"/>
       <c r="F55" s="15"/>
       <c r="G55" s="17"/>
-      <c r="H55" s="64"/>
+      <c r="H55" s="63"/>
     </row>
     <row r="56" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="15" t="s">
@@ -3220,7 +3266,7 @@
       <c r="E56" s="16"/>
       <c r="F56" s="15"/>
       <c r="G56" s="17"/>
-      <c r="H56" s="64"/>
+      <c r="H56" s="63"/>
     </row>
     <row r="57" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="15"/>
@@ -3228,7 +3274,7 @@
       <c r="E57" s="16"/>
       <c r="F57" s="15"/>
       <c r="G57" s="17"/>
-      <c r="H57" s="64"/>
+      <c r="H57" s="63"/>
     </row>
     <row r="58" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="20" t="s">
@@ -3247,7 +3293,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="17"/>
-      <c r="H58" s="64"/>
+      <c r="H58" s="63"/>
     </row>
     <row r="59" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="26" t="s">
@@ -3263,10 +3309,10 @@
         <v>15</v>
       </c>
       <c r="F59" s="29">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G59" s="50"/>
-      <c r="H59" s="64"/>
+      <c r="H59" s="63"/>
     </row>
     <row r="60" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="26"/>
@@ -3275,7 +3321,7 @@
       <c r="E60" s="28"/>
       <c r="F60" s="27"/>
       <c r="G60" s="50"/>
-      <c r="H60" s="64"/>
+      <c r="H60" s="63"/>
     </row>
     <row r="61" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="49"/>
@@ -3284,7 +3330,7 @@
       <c r="E61" s="28"/>
       <c r="F61" s="27"/>
       <c r="G61" s="17"/>
-      <c r="H61" s="64"/>
+      <c r="H61" s="63"/>
     </row>
     <row r="62" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="46" t="s">
@@ -3303,7 +3349,7 @@
         <v>2</v>
       </c>
       <c r="G62" s="45"/>
-      <c r="H62" s="64"/>
+      <c r="H62" s="63"/>
     </row>
     <row r="63" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
@@ -3321,7 +3367,7 @@
       <c r="F63" s="33">
         <v>3</v>
       </c>
-      <c r="H63" s="64"/>
+      <c r="H63" s="63"/>
     </row>
     <row r="64" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="46"/>
@@ -3329,7 +3375,7 @@
       <c r="D64" s="33"/>
       <c r="E64" s="34"/>
       <c r="F64" s="33"/>
-      <c r="H64" s="64"/>
+      <c r="H64" s="63"/>
     </row>
     <row r="65" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
@@ -3348,7 +3394,7 @@
         <v>10</v>
       </c>
       <c r="G65" s="45"/>
-      <c r="H65" s="64"/>
+      <c r="H65" s="63"/>
     </row>
     <row r="66" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
@@ -3364,10 +3410,10 @@
         <v>10</v>
       </c>
       <c r="F66" s="33">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G66" s="45"/>
-      <c r="H66" s="64"/>
+      <c r="H66" s="63"/>
     </row>
     <row r="67" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="46" t="s">
@@ -3385,7 +3431,7 @@
       <c r="F67" s="33">
         <v>9</v>
       </c>
-      <c r="H67" s="64"/>
+      <c r="H67" s="63"/>
     </row>
     <row r="68" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="46"/>
@@ -3394,7 +3440,7 @@
       <c r="E68" s="34"/>
       <c r="F68" s="33"/>
       <c r="G68" s="45"/>
-      <c r="H68" s="64"/>
+      <c r="H68" s="63"/>
     </row>
     <row r="69" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="46" t="s">
@@ -3410,9 +3456,9 @@
         <v>6</v>
       </c>
       <c r="F69" s="33">
-        <v>7</v>
-      </c>
-      <c r="H69" s="64"/>
+        <v>9</v>
+      </c>
+      <c r="H69" s="63"/>
     </row>
     <row r="70" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="46" t="s">
@@ -3431,7 +3477,7 @@
         <v>8</v>
       </c>
       <c r="G70" s="45"/>
-      <c r="H70" s="64"/>
+      <c r="H70" s="63"/>
     </row>
     <row r="71" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="46" t="s">
@@ -3447,9 +3493,9 @@
         <v>1</v>
       </c>
       <c r="F71" s="33">
-        <v>7</v>
-      </c>
-      <c r="H71" s="64"/>
+        <v>10</v>
+      </c>
+      <c r="H71" s="63"/>
     </row>
     <row r="72" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="46" t="s">
@@ -3465,9 +3511,9 @@
         <v>1</v>
       </c>
       <c r="F72" s="33">
-        <v>10</v>
-      </c>
-      <c r="H72" s="64"/>
+        <v>12</v>
+      </c>
+      <c r="H72" s="63"/>
     </row>
     <row r="73" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="46" t="s">
@@ -3479,7 +3525,7 @@
       <c r="D73" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E73" s="61">
+      <c r="E73" s="60">
         <v>1</v>
       </c>
       <c r="F73" s="46">
@@ -3488,7 +3534,7 @@
       <c r="G73" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H73" s="64"/>
+      <c r="H73" s="63"/>
     </row>
     <row r="74" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="46" t="s">
@@ -3500,7 +3546,7 @@
       <c r="D74" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="61" t="s">
+      <c r="E74" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F74" s="46">
@@ -3509,7 +3555,7 @@
       <c r="G74" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H74" s="67">
+      <c r="H74" s="66">
         <v>45604</v>
       </c>
     </row>
@@ -3523,7 +3569,7 @@
       <c r="D75" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E75" s="61" t="s">
+      <c r="E75" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F75" s="46">
@@ -3532,7 +3578,7 @@
       <c r="G75" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H75" s="67">
+      <c r="H75" s="66">
         <v>45628</v>
       </c>
     </row>
@@ -3546,7 +3592,7 @@
       <c r="D76" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E76" s="61" t="s">
+      <c r="E76" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F76" s="46">
@@ -3555,7 +3601,7 @@
       <c r="G76" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H76" s="67">
+      <c r="H76" s="66">
         <v>45649</v>
       </c>
     </row>
@@ -3573,10 +3619,10 @@
         <v>253</v>
       </c>
       <c r="F77" s="33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G77" s="45"/>
-      <c r="H77" s="67">
+      <c r="H77" s="66">
         <v>45670</v>
       </c>
     </row>
@@ -3595,7 +3641,7 @@
       <c r="E79" s="28"/>
       <c r="F79" s="29"/>
       <c r="G79" s="17"/>
-      <c r="H79" s="64"/>
+      <c r="H79" s="63"/>
     </row>
     <row r="80" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="15"/>
@@ -3606,10 +3652,10 @@
       </c>
       <c r="F80" s="43">
         <f>SUM(F62:F79)-SUM(F59:F61)</f>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G80" s="17"/>
-      <c r="H80" s="64"/>
+      <c r="H80" s="63"/>
     </row>
     <row r="81" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C81" s="15"/>
@@ -3617,7 +3663,7 @@
       <c r="E81" s="16"/>
       <c r="F81" s="15"/>
       <c r="G81" s="17"/>
-      <c r="H81" s="64"/>
+      <c r="H81" s="63"/>
     </row>
     <row r="82" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C82" s="15"/>
@@ -3625,7 +3671,7 @@
       <c r="E82" s="16"/>
       <c r="F82" s="15"/>
       <c r="G82" s="17"/>
-      <c r="H82" s="64"/>
+      <c r="H82" s="63"/>
     </row>
     <row r="83" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C83" s="15" t="s">
@@ -3637,7 +3683,7 @@
       <c r="E83" s="16"/>
       <c r="F83" s="15"/>
       <c r="G83" s="17"/>
-      <c r="H83" s="64"/>
+      <c r="H83" s="63"/>
     </row>
     <row r="84" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="15"/>
@@ -3645,7 +3691,7 @@
       <c r="E84" s="16"/>
       <c r="F84" s="15"/>
       <c r="G84" s="17"/>
-      <c r="H84" s="64"/>
+      <c r="H84" s="63"/>
     </row>
     <row r="85" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="20" t="s">
@@ -3664,7 +3710,7 @@
         <v>5</v>
       </c>
       <c r="G85" s="17"/>
-      <c r="H85" s="64"/>
+      <c r="H85" s="63"/>
     </row>
     <row r="86" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="26" t="s">
@@ -3676,16 +3722,16 @@
       <c r="D86" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="E86" s="62">
-        <v>1</v>
-      </c>
-      <c r="F86" s="63">
+      <c r="E86" s="61">
+        <v>1</v>
+      </c>
+      <c r="F86" s="62">
         <v>10</v>
       </c>
       <c r="G86" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H86" s="64"/>
+      <c r="H86" s="63"/>
     </row>
     <row r="87" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="49" t="s">
@@ -3701,10 +3747,10 @@
         <v>253</v>
       </c>
       <c r="F87" s="27">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G87" s="50"/>
-      <c r="H87" s="67">
+      <c r="H87" s="66">
         <v>45564</v>
       </c>
     </row>
@@ -3715,7 +3761,7 @@
       <c r="E88" s="28"/>
       <c r="F88" s="27"/>
       <c r="G88" s="17"/>
-      <c r="H88" s="64"/>
+      <c r="H88" s="63"/>
     </row>
     <row r="89" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="46" t="s">
@@ -3731,10 +3777,10 @@
         <v>10</v>
       </c>
       <c r="F89" s="33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G89" s="45"/>
-      <c r="H89" s="64"/>
+      <c r="H89" s="63"/>
     </row>
     <row r="90" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="46" t="s">
@@ -3746,7 +3792,7 @@
       <c r="D90" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="E90" s="61">
+      <c r="E90" s="60">
         <v>1</v>
       </c>
       <c r="F90" s="46">
@@ -3755,7 +3801,7 @@
       <c r="G90" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H90" s="64"/>
+      <c r="H90" s="63"/>
     </row>
     <row r="91" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="46" t="s">
@@ -3773,7 +3819,7 @@
       <c r="F91" s="33">
         <v>4</v>
       </c>
-      <c r="H91" s="67">
+      <c r="H91" s="66">
         <v>45534</v>
       </c>
     </row>
@@ -3787,7 +3833,7 @@
       <c r="D92" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E92" s="61">
+      <c r="E92" s="60">
         <v>1</v>
       </c>
       <c r="F92" s="46">
@@ -3813,7 +3859,7 @@
       <c r="F93" s="33">
         <v>3</v>
       </c>
-      <c r="H93" s="67">
+      <c r="H93" s="66">
         <v>45534</v>
       </c>
     </row>
@@ -3844,7 +3890,7 @@
       <c r="D95" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E95" s="61">
+      <c r="E95" s="60">
         <v>1</v>
       </c>
       <c r="F95" s="46">
@@ -3853,7 +3899,7 @@
       <c r="G95" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H95" s="64"/>
+      <c r="H95" s="63"/>
     </row>
     <row r="96" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="46" t="s">
@@ -3871,7 +3917,7 @@
       <c r="F96" s="33">
         <v>7</v>
       </c>
-      <c r="H96" s="67">
+      <c r="H96" s="66">
         <v>45526</v>
       </c>
     </row>
@@ -3889,9 +3935,9 @@
         <v>45</v>
       </c>
       <c r="F97" s="33">
-        <v>10</v>
-      </c>
-      <c r="H97" s="64"/>
+        <v>14</v>
+      </c>
+      <c r="H97" s="63"/>
     </row>
     <row r="98" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="46" t="s">
@@ -3903,7 +3949,7 @@
       <c r="D98" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="E98" s="61">
+      <c r="E98" s="60">
         <v>1</v>
       </c>
       <c r="F98" s="46">
@@ -3912,7 +3958,7 @@
       <c r="G98" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H98" s="64"/>
+      <c r="H98" s="63"/>
     </row>
     <row r="99" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="46" t="s">
@@ -3930,7 +3976,7 @@
       <c r="F99" s="33">
         <v>4</v>
       </c>
-      <c r="H99" s="67">
+      <c r="H99" s="66">
         <v>45566</v>
       </c>
     </row>
@@ -3944,7 +3990,7 @@
       <c r="D100" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E100" s="61">
+      <c r="E100" s="60">
         <v>1</v>
       </c>
       <c r="F100" s="46">
@@ -3964,7 +4010,7 @@
       <c r="D101" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="E101" s="61" t="s">
+      <c r="E101" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F101" s="46">
@@ -3973,7 +4019,7 @@
       <c r="G101" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H101" s="67">
+      <c r="H101" s="66">
         <v>45548</v>
       </c>
     </row>
@@ -3993,7 +4039,7 @@
       <c r="F102" s="33">
         <v>3</v>
       </c>
-      <c r="H102" s="67">
+      <c r="H102" s="66">
         <v>45588</v>
       </c>
     </row>
@@ -4007,7 +4053,7 @@
       <c r="D103" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E103" s="61">
+      <c r="E103" s="60">
         <v>1</v>
       </c>
       <c r="F103" s="46">
@@ -4016,7 +4062,7 @@
       <c r="G103" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H103" s="64"/>
+      <c r="H103" s="63"/>
     </row>
     <row r="104" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="46" t="s">
@@ -4028,7 +4074,7 @@
       <c r="D104" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="E104" s="61" t="s">
+      <c r="E104" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F104" s="46">
@@ -4037,7 +4083,7 @@
       <c r="G104" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H104" s="67">
+      <c r="H104" s="66">
         <v>45566</v>
       </c>
     </row>
@@ -4055,9 +4101,9 @@
         <v>253</v>
       </c>
       <c r="F105" s="33">
-        <v>6</v>
-      </c>
-      <c r="H105" s="67">
+        <v>7</v>
+      </c>
+      <c r="H105" s="66">
         <v>45627</v>
       </c>
     </row>
@@ -4075,10 +4121,10 @@
         <v>1</v>
       </c>
       <c r="F106" s="29">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G106" s="45"/>
-      <c r="H106" s="64"/>
+      <c r="H106" s="63"/>
     </row>
     <row r="107" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C107" s="15"/>
@@ -4089,7 +4135,7 @@
       </c>
       <c r="F107" s="43">
         <f>SUM(F89:F106)-SUM(F86:F88)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G107" s="17"/>
     </row>
@@ -4099,7 +4145,7 @@
       <c r="E108" s="16"/>
       <c r="F108" s="15"/>
       <c r="G108" s="17"/>
-      <c r="H108" s="64"/>
+      <c r="H108" s="63"/>
     </row>
     <row r="109" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C109" s="15"/>
@@ -4107,7 +4153,7 @@
       <c r="E109" s="16"/>
       <c r="F109" s="15"/>
       <c r="G109" s="17"/>
-      <c r="H109" s="64"/>
+      <c r="H109" s="63"/>
     </row>
     <row r="110" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C110" s="15" t="s">
@@ -4119,7 +4165,7 @@
       <c r="E110" s="16"/>
       <c r="F110" s="15"/>
       <c r="G110" s="17"/>
-      <c r="H110" s="64"/>
+      <c r="H110" s="63"/>
     </row>
     <row r="111" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="15"/>
@@ -4127,7 +4173,7 @@
       <c r="E111" s="16"/>
       <c r="F111" s="15"/>
       <c r="G111" s="17"/>
-      <c r="H111" s="64"/>
+      <c r="H111" s="63"/>
     </row>
     <row r="112" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B112" s="20" t="s">
@@ -4146,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="G112" s="17"/>
-      <c r="H112" s="64"/>
+      <c r="H112" s="63"/>
     </row>
     <row r="113" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="26" t="s">
@@ -4158,16 +4204,16 @@
       <c r="D113" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E113" s="62">
+      <c r="E113" s="61">
         <v>5</v>
       </c>
-      <c r="F113" s="63">
+      <c r="F113" s="62">
         <v>34</v>
       </c>
       <c r="G113" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H113" s="64"/>
+      <c r="H113" s="63"/>
     </row>
     <row r="114" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="49" t="s">
@@ -4183,10 +4229,10 @@
         <v>253</v>
       </c>
       <c r="F114" s="27">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G114" s="50"/>
-      <c r="H114" s="67">
+      <c r="H114" s="66">
         <v>45702</v>
       </c>
     </row>
@@ -4197,7 +4243,7 @@
       <c r="E115" s="28"/>
       <c r="F115" s="27"/>
       <c r="G115" s="17"/>
-      <c r="H115" s="64"/>
+      <c r="H115" s="63"/>
     </row>
     <row r="116" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="46" t="s">
@@ -4213,9 +4259,9 @@
         <v>3</v>
       </c>
       <c r="F116" s="33">
-        <v>3</v>
-      </c>
-      <c r="H116" s="64"/>
+        <v>4</v>
+      </c>
+      <c r="H116" s="63"/>
     </row>
     <row r="117" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="46" t="s">
@@ -4231,10 +4277,10 @@
         <v>1</v>
       </c>
       <c r="F117" s="33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G117" s="45"/>
-      <c r="H117" s="64"/>
+      <c r="H117" s="63"/>
     </row>
     <row r="118" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="46" t="s">
@@ -4246,7 +4292,7 @@
       <c r="D118" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="E118" s="61">
+      <c r="E118" s="60">
         <v>1</v>
       </c>
       <c r="F118" s="46">
@@ -4255,7 +4301,7 @@
       <c r="G118" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H118" s="64"/>
+      <c r="H118" s="63"/>
     </row>
     <row r="119" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="46" t="s">
@@ -4267,7 +4313,7 @@
       <c r="D119" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="E119" s="61" t="s">
+      <c r="E119" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F119" s="46">
@@ -4276,7 +4322,7 @@
       <c r="G119" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H119" s="67">
+      <c r="H119" s="66">
         <v>45551</v>
       </c>
     </row>
@@ -4294,9 +4340,9 @@
         <v>253</v>
       </c>
       <c r="F120" s="33">
-        <v>9</v>
-      </c>
-      <c r="H120" s="67">
+        <v>10</v>
+      </c>
+      <c r="H120" s="66">
         <v>45592</v>
       </c>
     </row>
@@ -4310,7 +4356,7 @@
       <c r="D121" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="E121" s="61">
+      <c r="E121" s="60">
         <v>1</v>
       </c>
       <c r="F121" s="46">
@@ -4330,7 +4376,7 @@
       <c r="D122" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="E122" s="61" t="s">
+      <c r="E122" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F122" s="46">
@@ -4339,7 +4385,7 @@
       <c r="G122" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H122" s="67">
+      <c r="H122" s="66">
         <v>45529</v>
       </c>
     </row>
@@ -4359,7 +4405,7 @@
       <c r="F123" s="33">
         <v>2</v>
       </c>
-      <c r="H123" s="67">
+      <c r="H123" s="66">
         <v>45653</v>
       </c>
     </row>
@@ -4379,7 +4425,7 @@
       <c r="F124" s="33">
         <v>4</v>
       </c>
-      <c r="H124" s="67"/>
+      <c r="H124" s="66"/>
     </row>
     <row r="125" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="46" t="s">
@@ -4395,9 +4441,9 @@
         <v>7</v>
       </c>
       <c r="F125" s="33">
-        <v>15</v>
-      </c>
-      <c r="H125" s="67"/>
+        <v>16</v>
+      </c>
+      <c r="H125" s="66"/>
     </row>
     <row r="126" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="46" t="s">
@@ -4413,9 +4459,9 @@
         <v>15</v>
       </c>
       <c r="F126" s="33">
-        <v>7</v>
-      </c>
-      <c r="H126" s="67"/>
+        <v>8</v>
+      </c>
+      <c r="H126" s="66"/>
     </row>
     <row r="127" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="46" t="s">
@@ -4427,7 +4473,7 @@
       <c r="D127" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="E127" s="61">
+      <c r="E127" s="60">
         <v>39</v>
       </c>
       <c r="F127" s="46">
@@ -4436,7 +4482,7 @@
       <c r="G127" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H127" s="67"/>
+      <c r="H127" s="66"/>
     </row>
     <row r="128" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="46" t="s">
@@ -4452,10 +4498,10 @@
         <v>253</v>
       </c>
       <c r="F128" s="33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G128" s="45"/>
-      <c r="H128" s="67">
+      <c r="H128" s="66">
         <v>45698</v>
       </c>
     </row>
@@ -4469,7 +4515,7 @@
       <c r="D129" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="E129" s="61">
+      <c r="E129" s="60">
         <v>12</v>
       </c>
       <c r="F129" s="46">
@@ -4478,7 +4524,7 @@
       <c r="G129" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H129" s="64"/>
+      <c r="H129" s="63"/>
     </row>
     <row r="130" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="46" t="s">
@@ -4496,7 +4542,7 @@
       <c r="F130" s="33">
         <v>14</v>
       </c>
-      <c r="H130" s="67">
+      <c r="H130" s="66">
         <v>45563</v>
       </c>
     </row>
@@ -4510,7 +4556,7 @@
       <c r="D131" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="E131" s="61">
+      <c r="E131" s="60">
         <v>11</v>
       </c>
       <c r="F131" s="46">
@@ -4519,7 +4565,7 @@
       <c r="G131" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H131" s="64"/>
+      <c r="H131" s="63"/>
     </row>
     <row r="132" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="46" t="s">
@@ -4531,7 +4577,7 @@
       <c r="D132" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="E132" s="61" t="s">
+      <c r="E132" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F132" s="46">
@@ -4540,7 +4586,7 @@
       <c r="G132" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H132" s="67">
+      <c r="H132" s="66">
         <v>45556</v>
       </c>
     </row>
@@ -4558,10 +4604,10 @@
         <v>253</v>
       </c>
       <c r="F133" s="29">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G133" s="17"/>
-      <c r="H133" s="67">
+      <c r="H133" s="66">
         <v>45632</v>
       </c>
     </row>
@@ -4574,10 +4620,10 @@
       </c>
       <c r="F134" s="43">
         <f>SUM(F116:F133)-SUM(F113:F115)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G134" s="17"/>
-      <c r="H134" s="64"/>
+      <c r="H134" s="63"/>
     </row>
     <row r="135" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C135" s="15"/>
@@ -4585,7 +4631,7 @@
       <c r="E135" s="16"/>
       <c r="F135" s="15"/>
       <c r="G135" s="17"/>
-      <c r="H135" s="64"/>
+      <c r="H135" s="63"/>
     </row>
     <row r="136" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C136" s="15"/>
@@ -4593,7 +4639,7 @@
       <c r="E136" s="16"/>
       <c r="F136" s="15"/>
       <c r="G136" s="17"/>
-      <c r="H136" s="64"/>
+      <c r="H136" s="63"/>
     </row>
     <row r="137" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C137" s="15" t="s">
@@ -4605,7 +4651,7 @@
       <c r="E137" s="16"/>
       <c r="F137" s="15"/>
       <c r="G137" s="17"/>
-      <c r="H137" s="64"/>
+      <c r="H137" s="63"/>
     </row>
     <row r="138" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C138" s="15"/>
@@ -4613,7 +4659,7 @@
       <c r="E138" s="16"/>
       <c r="F138" s="15"/>
       <c r="G138" s="17"/>
-      <c r="H138" s="64"/>
+      <c r="H138" s="63"/>
     </row>
     <row r="139" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B139" s="20" t="s">
@@ -4632,7 +4678,7 @@
         <v>5</v>
       </c>
       <c r="G139" s="50"/>
-      <c r="H139" s="64"/>
+      <c r="H139" s="63"/>
     </row>
     <row r="140" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="26" t="s">
@@ -4644,16 +4690,16 @@
       <c r="D140" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="E140" s="62">
-        <v>1</v>
-      </c>
-      <c r="F140" s="63">
+      <c r="E140" s="61">
+        <v>1</v>
+      </c>
+      <c r="F140" s="62">
         <v>7</v>
       </c>
       <c r="G140" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H140" s="64"/>
+      <c r="H140" s="63"/>
     </row>
     <row r="141" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="49" t="s">
@@ -4669,10 +4715,10 @@
         <v>253</v>
       </c>
       <c r="F141" s="27">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G141" s="50"/>
-      <c r="H141" s="67">
+      <c r="H141" s="66">
         <v>45529</v>
       </c>
     </row>
@@ -4683,7 +4729,7 @@
       <c r="E142" s="28"/>
       <c r="F142" s="27"/>
       <c r="G142" s="45"/>
-      <c r="H142" s="64"/>
+      <c r="H142" s="63"/>
     </row>
     <row r="143" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="46" t="s">
@@ -4699,9 +4745,9 @@
         <v>1</v>
       </c>
       <c r="F143" s="33">
-        <v>0</v>
-      </c>
-      <c r="H143" s="64"/>
+        <v>1</v>
+      </c>
+      <c r="H143" s="63"/>
     </row>
     <row r="144" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="46" t="s">
@@ -4719,7 +4765,7 @@
       <c r="F144" s="33">
         <v>1</v>
       </c>
-      <c r="H144" s="64"/>
+      <c r="H144" s="63"/>
     </row>
     <row r="145" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="46" t="s">
@@ -4731,7 +4777,7 @@
       <c r="D145" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E145" s="61">
+      <c r="E145" s="60">
         <v>1</v>
       </c>
       <c r="F145" s="46">
@@ -4740,7 +4786,7 @@
       <c r="G145" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H145" s="64"/>
+      <c r="H145" s="63"/>
     </row>
     <row r="146" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="46" t="s">
@@ -4758,7 +4804,7 @@
       <c r="F146" s="33">
         <v>8</v>
       </c>
-      <c r="H146" s="67">
+      <c r="H146" s="66">
         <v>45604</v>
       </c>
     </row>
@@ -4772,7 +4818,7 @@
       <c r="D147" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E147" s="61">
+      <c r="E147" s="60">
         <v>1</v>
       </c>
       <c r="F147" s="46">
@@ -4781,25 +4827,25 @@
       <c r="G147" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H147" s="64"/>
+      <c r="H147" s="63"/>
     </row>
     <row r="148" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C148" s="33" t="s">
+      <c r="C148" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="D148" s="33" t="s">
+      <c r="D148" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="E148" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="F148" s="33">
-        <v>1</v>
-      </c>
-      <c r="H148" s="67">
+      <c r="E148" s="60" t="s">
+        <v>253</v>
+      </c>
+      <c r="F148" s="46">
+        <v>1</v>
+      </c>
+      <c r="H148" s="66">
         <v>45692</v>
       </c>
     </row>
@@ -4807,49 +4853,62 @@
       <c r="B149" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C149" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="D149" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E149" s="61">
-        <v>1</v>
-      </c>
-      <c r="F149" s="46">
-        <v>1</v>
-      </c>
-      <c r="G149" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="H149" s="64"/>
+      <c r="C149" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="D149" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E149" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F149" s="33">
+        <v>0</v>
+      </c>
+      <c r="H149" s="66">
+        <v>45744</v>
+      </c>
     </row>
     <row r="150" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C150" s="33" t="s">
+      <c r="C150" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="D150" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E150" s="60">
+        <v>1</v>
+      </c>
+      <c r="F150" s="46">
+        <v>1</v>
+      </c>
+      <c r="G150" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="H150" s="63"/>
+    </row>
+    <row r="151" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="D150" s="33" t="s">
+      <c r="D151" s="33" t="s">
         <v>281</v>
       </c>
-      <c r="E150" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="F150" s="33">
+      <c r="E151" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="F151" s="33">
         <v>5</v>
       </c>
-      <c r="H150" s="67">
+      <c r="H151" s="66">
         <v>45564</v>
       </c>
-    </row>
-    <row r="151" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="53"/>
-      <c r="C151" s="53"/>
-      <c r="D151" s="53"/>
-      <c r="E151" s="60"/>
-      <c r="F151" s="53"/>
     </row>
     <row r="152" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="46" t="s">
@@ -4865,10 +4924,10 @@
         <v>80</v>
       </c>
       <c r="F152" s="33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G152" s="45"/>
-      <c r="H152" s="64"/>
+      <c r="H152" s="63"/>
     </row>
     <row r="153" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="46" t="s">
@@ -4880,7 +4939,7 @@
       <c r="D153" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="E153" s="61">
+      <c r="E153" s="60">
         <v>2</v>
       </c>
       <c r="F153" s="46">
@@ -4889,7 +4948,7 @@
       <c r="G153" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H153" s="64"/>
+      <c r="H153" s="63"/>
     </row>
     <row r="154" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="46" t="s">
@@ -4901,7 +4960,7 @@
       <c r="D154" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="E154" s="61" t="s">
+      <c r="E154" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F154" s="46">
@@ -4910,7 +4969,7 @@
       <c r="G154" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H154" s="67">
+      <c r="H154" s="66">
         <v>45552</v>
       </c>
     </row>
@@ -4928,9 +4987,9 @@
         <v>253</v>
       </c>
       <c r="F155" s="33">
-        <v>11</v>
-      </c>
-      <c r="H155" s="67">
+        <v>13</v>
+      </c>
+      <c r="H155" s="66">
         <v>45592</v>
       </c>
     </row>
@@ -4944,7 +5003,7 @@
       <c r="D156" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="E156" s="61">
+      <c r="E156" s="60">
         <v>1</v>
       </c>
       <c r="F156" s="46">
@@ -4953,7 +5012,7 @@
       <c r="G156" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H156" s="67"/>
+      <c r="H156" s="66"/>
     </row>
     <row r="157" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="46" t="s">
@@ -4969,9 +5028,9 @@
         <v>253</v>
       </c>
       <c r="F157" s="33">
-        <v>12</v>
-      </c>
-      <c r="H157" s="67">
+        <v>13</v>
+      </c>
+      <c r="H157" s="66">
         <v>45552</v>
       </c>
     </row>
@@ -4985,7 +5044,7 @@
       <c r="D158" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="E158" s="61">
+      <c r="E158" s="60">
         <v>6</v>
       </c>
       <c r="F158" s="46">
@@ -4994,7 +5053,7 @@
       <c r="G158" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H158" s="67"/>
+      <c r="H158" s="66"/>
     </row>
     <row r="159" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="46" t="s">
@@ -5010,9 +5069,9 @@
         <v>253</v>
       </c>
       <c r="F159" s="33">
-        <v>9</v>
-      </c>
-      <c r="H159" s="67">
+        <v>11</v>
+      </c>
+      <c r="H159" s="66">
         <v>45564</v>
       </c>
     </row>
@@ -5030,10 +5089,10 @@
         <v>1</v>
       </c>
       <c r="F160" s="29">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G160" s="17"/>
-      <c r="H160" s="64"/>
+      <c r="H160" s="63"/>
     </row>
     <row r="161" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C161" s="15"/>
@@ -5044,10 +5103,10 @@
       </c>
       <c r="F161" s="43">
         <f>SUM(F143:F160)-SUM(F140:F142)</f>
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G161" s="17"/>
-      <c r="H161" s="64"/>
+      <c r="H161" s="63"/>
     </row>
     <row r="162" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C162" s="15"/>
@@ -5055,7 +5114,7 @@
       <c r="E162" s="16"/>
       <c r="F162" s="15"/>
       <c r="G162" s="17"/>
-      <c r="H162" s="64"/>
+      <c r="H162" s="63"/>
     </row>
     <row r="163" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C163" s="15"/>
@@ -5063,7 +5122,7 @@
       <c r="E163" s="16"/>
       <c r="F163" s="15"/>
       <c r="G163" s="17"/>
-      <c r="H163" s="64"/>
+      <c r="H163" s="63"/>
     </row>
     <row r="164" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C164" s="15" t="s">
@@ -5075,7 +5134,7 @@
       <c r="E164" s="16"/>
       <c r="F164" s="15"/>
       <c r="G164" s="17"/>
-      <c r="H164" s="64"/>
+      <c r="H164" s="63"/>
     </row>
     <row r="165" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C165" s="15"/>
@@ -5083,7 +5142,7 @@
       <c r="E165" s="16"/>
       <c r="F165" s="15"/>
       <c r="G165" s="17"/>
-      <c r="H165" s="64"/>
+      <c r="H165" s="63"/>
     </row>
     <row r="166" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="20" t="s">
@@ -5102,7 +5161,7 @@
         <v>5</v>
       </c>
       <c r="G166" s="50"/>
-      <c r="H166" s="64"/>
+      <c r="H166" s="63"/>
     </row>
     <row r="167" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="26" t="s">
@@ -5114,16 +5173,16 @@
       <c r="D167" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E167" s="62">
+      <c r="E167" s="61">
         <v>7</v>
       </c>
-      <c r="F167" s="63">
+      <c r="F167" s="62">
         <v>43</v>
       </c>
       <c r="G167" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H167" s="64"/>
+      <c r="H167" s="63"/>
     </row>
     <row r="168" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="49" t="s">
@@ -5139,10 +5198,10 @@
         <v>253</v>
       </c>
       <c r="F168" s="27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G168" s="50"/>
-      <c r="H168" s="67">
+      <c r="H168" s="66">
         <v>45715</v>
       </c>
     </row>
@@ -5153,7 +5212,7 @@
       <c r="E169" s="28"/>
       <c r="F169" s="27"/>
       <c r="G169" s="47"/>
-      <c r="H169" s="64"/>
+      <c r="H169" s="63"/>
     </row>
     <row r="170" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="46" t="s">
@@ -5169,9 +5228,9 @@
         <v>3</v>
       </c>
       <c r="F170" s="33">
-        <v>1</v>
-      </c>
-      <c r="H170" s="64"/>
+        <v>2</v>
+      </c>
+      <c r="H170" s="63"/>
     </row>
     <row r="171" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="46" t="s">
@@ -5190,7 +5249,7 @@
         <v>2</v>
       </c>
       <c r="G171" s="45"/>
-      <c r="H171" s="64"/>
+      <c r="H171" s="63"/>
     </row>
     <row r="172" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="46" t="s">
@@ -5202,7 +5261,7 @@
       <c r="D172" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="E172" s="61">
+      <c r="E172" s="60">
         <v>9</v>
       </c>
       <c r="F172" s="46">
@@ -5211,7 +5270,7 @@
       <c r="G172" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H172" s="64"/>
+      <c r="H172" s="63"/>
     </row>
     <row r="173" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="46" t="s">
@@ -5227,9 +5286,9 @@
         <v>253</v>
       </c>
       <c r="F173" s="33">
-        <v>6</v>
-      </c>
-      <c r="H173" s="67">
+        <v>7</v>
+      </c>
+      <c r="H173" s="66">
         <v>45601</v>
       </c>
     </row>
@@ -5243,7 +5302,7 @@
       <c r="D174" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E174" s="61">
+      <c r="E174" s="60">
         <v>15</v>
       </c>
       <c r="F174" s="46">
@@ -5269,7 +5328,7 @@
       <c r="F175" s="33">
         <v>0</v>
       </c>
-      <c r="H175" s="67">
+      <c r="H175" s="66">
         <v>45700</v>
       </c>
     </row>
@@ -5283,7 +5342,7 @@
       <c r="D176" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="E176" s="61">
+      <c r="E176" s="60">
         <v>1</v>
       </c>
       <c r="F176" s="46">
@@ -5292,7 +5351,7 @@
       <c r="G176" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H176" s="64"/>
+      <c r="H176" s="63"/>
     </row>
     <row r="177" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="46" t="s">
@@ -5308,9 +5367,9 @@
         <v>253</v>
       </c>
       <c r="F177" s="33">
-        <v>7</v>
-      </c>
-      <c r="H177" s="67">
+        <v>8</v>
+      </c>
+      <c r="H177" s="66">
         <v>45526</v>
       </c>
     </row>
@@ -5328,7 +5387,7 @@
         <v>3</v>
       </c>
       <c r="F178" s="33">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -5341,7 +5400,7 @@
       <c r="D179" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="E179" s="61">
+      <c r="E179" s="60">
         <v>4</v>
       </c>
       <c r="F179" s="46">
@@ -5350,7 +5409,7 @@
       <c r="G179" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H179" s="64"/>
+      <c r="H179" s="63"/>
     </row>
     <row r="180" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="46" t="s">
@@ -5368,7 +5427,7 @@
       <c r="F180" s="33">
         <v>10</v>
       </c>
-      <c r="H180" s="67">
+      <c r="H180" s="66">
         <v>45601</v>
       </c>
     </row>
@@ -5382,7 +5441,7 @@
       <c r="D181" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="E181" s="61">
+      <c r="E181" s="60">
         <v>5</v>
       </c>
       <c r="F181" s="46">
@@ -5391,7 +5450,7 @@
       <c r="G181" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H181" s="67"/>
+      <c r="H181" s="66"/>
     </row>
     <row r="182" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="46" t="s">
@@ -5409,7 +5468,7 @@
       <c r="F182" s="33">
         <v>0</v>
       </c>
-      <c r="H182" s="67">
+      <c r="H182" s="66">
         <v>45664</v>
       </c>
     </row>
@@ -5423,7 +5482,7 @@
       <c r="D183" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="E183" s="61">
+      <c r="E183" s="60">
         <v>38</v>
       </c>
       <c r="F183" s="46">
@@ -5432,7 +5491,7 @@
       <c r="G183" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H183" s="67"/>
+      <c r="H183" s="66"/>
     </row>
     <row r="184" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="46" t="s">
@@ -5450,7 +5509,7 @@
       <c r="F184" s="33">
         <v>3</v>
       </c>
-      <c r="H184" s="67">
+      <c r="H184" s="66">
         <v>45676</v>
       </c>
     </row>
@@ -5464,7 +5523,7 @@
       <c r="D185" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="E185" s="61">
+      <c r="E185" s="60">
         <v>10</v>
       </c>
       <c r="F185" s="46">
@@ -5484,7 +5543,7 @@
       <c r="D186" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="E186" s="61" t="s">
+      <c r="E186" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F186" s="53">
@@ -5493,7 +5552,7 @@
       <c r="G186" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H186" s="67">
+      <c r="H186" s="66">
         <v>45565</v>
       </c>
     </row>
@@ -5514,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="G187" s="17"/>
-      <c r="H187" s="67">
+      <c r="H187" s="66">
         <v>45692</v>
       </c>
     </row>
@@ -5527,10 +5586,10 @@
       </c>
       <c r="F188" s="43">
         <f>SUM(F170:F187)-SUM(F167:F169)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G188" s="17"/>
-      <c r="H188" s="64"/>
+      <c r="H188" s="63"/>
     </row>
     <row r="189" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C189" s="15"/>
@@ -5538,7 +5597,7 @@
       <c r="E189" s="16"/>
       <c r="F189" s="15"/>
       <c r="G189" s="17"/>
-      <c r="H189" s="64"/>
+      <c r="H189" s="63"/>
     </row>
     <row r="190" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C190" s="15"/>
@@ -5546,7 +5605,7 @@
       <c r="E190" s="16"/>
       <c r="F190" s="15"/>
       <c r="G190" s="17"/>
-      <c r="H190" s="64"/>
+      <c r="H190" s="63"/>
     </row>
     <row r="191" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C191" s="15" t="s">
@@ -5558,7 +5617,7 @@
       <c r="E191" s="16"/>
       <c r="F191" s="15"/>
       <c r="G191" s="17"/>
-      <c r="H191" s="64"/>
+      <c r="H191" s="63"/>
     </row>
     <row r="192" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C192" s="15"/>
@@ -5566,7 +5625,7 @@
       <c r="E192" s="16"/>
       <c r="F192" s="15"/>
       <c r="G192" s="17"/>
-      <c r="H192" s="64"/>
+      <c r="H192" s="63"/>
     </row>
     <row r="193" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B193" s="20" t="s">
@@ -5585,7 +5644,7 @@
         <v>5</v>
       </c>
       <c r="G193" s="50"/>
-      <c r="H193" s="64"/>
+      <c r="H193" s="63"/>
     </row>
     <row r="194" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="26" t="s">
@@ -5601,10 +5660,10 @@
         <v>4</v>
       </c>
       <c r="F194" s="29">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G194" s="50"/>
-      <c r="H194" s="64"/>
+      <c r="H194" s="63"/>
     </row>
     <row r="195" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="26"/>
@@ -5613,7 +5672,7 @@
       <c r="E195" s="28"/>
       <c r="F195" s="27"/>
       <c r="G195" s="17"/>
-      <c r="H195" s="64"/>
+      <c r="H195" s="63"/>
     </row>
     <row r="196" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="49"/>
@@ -5622,7 +5681,7 @@
       <c r="E196" s="28"/>
       <c r="F196" s="27"/>
       <c r="G196" s="45"/>
-      <c r="H196" s="64"/>
+      <c r="H196" s="63"/>
     </row>
     <row r="197" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="46" t="s">
@@ -5634,7 +5693,7 @@
       <c r="D197" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="E197" s="61">
+      <c r="E197" s="60">
         <v>3</v>
       </c>
       <c r="F197" s="46">
@@ -5643,7 +5702,7 @@
       <c r="G197" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H197" s="64"/>
+      <c r="H197" s="63"/>
     </row>
     <row r="198" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="46" t="s">
@@ -5661,7 +5720,7 @@
       <c r="F198" s="33">
         <v>3</v>
       </c>
-      <c r="H198" s="67">
+      <c r="H198" s="66">
         <v>45564</v>
       </c>
     </row>
@@ -5682,7 +5741,7 @@
         <v>1</v>
       </c>
       <c r="G199" s="45"/>
-      <c r="H199" s="64"/>
+      <c r="H199" s="63"/>
     </row>
     <row r="200" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="46"/>
@@ -5691,7 +5750,7 @@
       <c r="E200" s="34"/>
       <c r="F200" s="33"/>
       <c r="G200" s="45"/>
-      <c r="H200" s="64"/>
+      <c r="H200" s="63"/>
     </row>
     <row r="201" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="46" t="s">
@@ -5707,9 +5766,9 @@
         <v>23</v>
       </c>
       <c r="F201" s="33">
-        <v>9</v>
-      </c>
-      <c r="H201" s="64"/>
+        <v>10</v>
+      </c>
+      <c r="H201" s="63"/>
     </row>
     <row r="202" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="46" t="s">
@@ -5728,7 +5787,7 @@
         <v>5</v>
       </c>
       <c r="G202" s="45"/>
-      <c r="H202" s="64"/>
+      <c r="H202" s="63"/>
     </row>
     <row r="203" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="46" t="s">
@@ -5740,7 +5799,7 @@
       <c r="D203" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="E203" s="61">
+      <c r="E203" s="60">
         <v>2</v>
       </c>
       <c r="F203" s="46">
@@ -5749,7 +5808,7 @@
       <c r="G203" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H203" s="64"/>
+      <c r="H203" s="63"/>
     </row>
     <row r="204" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="46" t="s">
@@ -5768,7 +5827,7 @@
         <v>3</v>
       </c>
       <c r="G204" s="45"/>
-      <c r="H204" s="67">
+      <c r="H204" s="66">
         <v>45515</v>
       </c>
     </row>
@@ -5776,9 +5835,9 @@
       <c r="B205" s="53"/>
       <c r="C205" s="53"/>
       <c r="D205" s="53"/>
-      <c r="E205" s="60"/>
+      <c r="E205" s="59"/>
       <c r="F205" s="53"/>
-      <c r="H205" s="64"/>
+      <c r="H205" s="63"/>
     </row>
     <row r="206" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="46" t="s">
@@ -5797,7 +5856,7 @@
         <v>11</v>
       </c>
       <c r="G206" s="45"/>
-      <c r="H206" s="64"/>
+      <c r="H206" s="63"/>
     </row>
     <row r="207" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="46" t="s">
@@ -5813,9 +5872,9 @@
         <v>4</v>
       </c>
       <c r="F207" s="33">
-        <v>7</v>
-      </c>
-      <c r="H207" s="64"/>
+        <v>8</v>
+      </c>
+      <c r="H207" s="63"/>
     </row>
     <row r="208" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="46" t="s">
@@ -5833,7 +5892,7 @@
       <c r="F208" s="33">
         <v>7</v>
       </c>
-      <c r="H208" s="64"/>
+      <c r="H208" s="63"/>
     </row>
     <row r="209" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="46" t="s">
@@ -5863,7 +5922,7 @@
       <c r="D210" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="E210" s="61">
+      <c r="E210" s="60">
         <v>15</v>
       </c>
       <c r="F210" s="46">
@@ -5872,7 +5931,7 @@
       <c r="G210" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H210" s="64"/>
+      <c r="H210" s="63"/>
     </row>
     <row r="211" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="46" t="s">
@@ -5888,9 +5947,9 @@
         <v>253</v>
       </c>
       <c r="F211" s="33">
-        <v>4</v>
-      </c>
-      <c r="H211" s="67">
+        <v>5</v>
+      </c>
+      <c r="H211" s="66">
         <v>45535</v>
       </c>
     </row>
@@ -5900,7 +5959,7 @@
       <c r="D212" s="33"/>
       <c r="E212" s="34"/>
       <c r="F212" s="33"/>
-      <c r="H212" s="64"/>
+      <c r="H212" s="63"/>
     </row>
     <row r="213" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="46"/>
@@ -5909,7 +5968,7 @@
       <c r="E213" s="34"/>
       <c r="F213" s="33"/>
       <c r="G213" s="45"/>
-      <c r="H213" s="64"/>
+      <c r="H213" s="63"/>
     </row>
     <row r="214" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B214" s="48"/>
@@ -5918,7 +5977,7 @@
       <c r="E214" s="28"/>
       <c r="F214" s="29"/>
       <c r="G214" s="17"/>
-      <c r="H214" s="64"/>
+      <c r="H214" s="63"/>
     </row>
     <row r="215" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C215" s="15"/>
@@ -5929,10 +5988,10 @@
       </c>
       <c r="F215" s="43">
         <f>SUM(F197:F214)-SUM(F194:F196)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G215" s="17"/>
-      <c r="H215" s="64"/>
+      <c r="H215" s="63"/>
     </row>
     <row r="216" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C216" s="15"/>
@@ -5940,7 +5999,7 @@
       <c r="E216" s="16"/>
       <c r="F216" s="15"/>
       <c r="G216" s="17"/>
-      <c r="H216" s="64"/>
+      <c r="H216" s="63"/>
     </row>
     <row r="217" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C217" s="15"/>
@@ -5948,7 +6007,7 @@
       <c r="E217" s="16"/>
       <c r="F217" s="15"/>
       <c r="G217" s="17"/>
-      <c r="H217" s="64"/>
+      <c r="H217" s="63"/>
     </row>
     <row r="218" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C218" s="15" t="s">
@@ -5960,7 +6019,7 @@
       <c r="E218" s="16"/>
       <c r="F218" s="15"/>
       <c r="G218" s="17"/>
-      <c r="H218" s="64"/>
+      <c r="H218" s="63"/>
     </row>
     <row r="219" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C219" s="15"/>
@@ -5968,7 +6027,7 @@
       <c r="E219" s="16"/>
       <c r="F219" s="15"/>
       <c r="G219" s="17"/>
-      <c r="H219" s="64"/>
+      <c r="H219" s="63"/>
     </row>
     <row r="220" spans="2:8" ht="12.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B220" s="20" t="s">
@@ -5987,7 +6046,7 @@
         <v>5</v>
       </c>
       <c r="G220" s="50"/>
-      <c r="H220" s="64"/>
+      <c r="H220" s="63"/>
     </row>
     <row r="221" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B221" s="26" t="s">
@@ -5999,16 +6058,16 @@
       <c r="D221" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="E221" s="62">
-        <v>1</v>
-      </c>
-      <c r="F221" s="63">
+      <c r="E221" s="61">
+        <v>1</v>
+      </c>
+      <c r="F221" s="62">
         <v>30</v>
       </c>
       <c r="G221" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="H221" s="64"/>
+      <c r="H221" s="63"/>
     </row>
     <row r="222" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="49" t="s">
@@ -6024,10 +6083,10 @@
         <v>253</v>
       </c>
       <c r="F222" s="27">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G222" s="50"/>
-      <c r="H222" s="67">
+      <c r="H222" s="66">
         <v>45682</v>
       </c>
     </row>
@@ -6038,7 +6097,7 @@
       <c r="E223" s="28"/>
       <c r="F223" s="27"/>
       <c r="G223" s="45"/>
-      <c r="H223" s="64"/>
+      <c r="H223" s="63"/>
     </row>
     <row r="224" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="46" t="s">
@@ -6056,7 +6115,7 @@
       <c r="F224" s="33">
         <v>5</v>
       </c>
-      <c r="H224" s="64"/>
+      <c r="H224" s="63"/>
     </row>
     <row r="225" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B225" s="46" t="s">
@@ -6075,7 +6134,7 @@
         <v>1</v>
       </c>
       <c r="G225" s="45"/>
-      <c r="H225" s="64"/>
+      <c r="H225" s="63"/>
     </row>
     <row r="226" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="46" t="s">
@@ -6087,7 +6146,7 @@
       <c r="D226" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="E226" s="61">
+      <c r="E226" s="60">
         <v>16</v>
       </c>
       <c r="F226" s="46">
@@ -6096,7 +6155,7 @@
       <c r="G226" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H226" s="64"/>
+      <c r="H226" s="63"/>
     </row>
     <row r="227" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="46" t="s">
@@ -6108,7 +6167,7 @@
       <c r="D227" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="E227" s="61" t="s">
+      <c r="E227" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F227" s="46">
@@ -6117,7 +6176,7 @@
       <c r="G227" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H227" s="67">
+      <c r="H227" s="66">
         <v>45529</v>
       </c>
     </row>
@@ -6135,9 +6194,9 @@
         <v>253</v>
       </c>
       <c r="F228" s="33">
-        <v>4</v>
-      </c>
-      <c r="H228" s="67">
+        <v>5</v>
+      </c>
+      <c r="H228" s="66">
         <v>45590</v>
       </c>
     </row>
@@ -6151,7 +6210,7 @@
       <c r="D229" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E229" s="61">
+      <c r="E229" s="60">
         <v>12</v>
       </c>
       <c r="F229" s="46">
@@ -6160,7 +6219,7 @@
       <c r="G229" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H229" s="64"/>
+      <c r="H229" s="63"/>
     </row>
     <row r="230" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B230" s="46" t="s">
@@ -6178,7 +6237,7 @@
       <c r="F230" s="33">
         <v>4</v>
       </c>
-      <c r="H230" s="67">
+      <c r="H230" s="66">
         <v>45590</v>
       </c>
     </row>
@@ -6192,7 +6251,7 @@
       <c r="D231" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="E231" s="61">
+      <c r="E231" s="60">
         <v>3</v>
       </c>
       <c r="F231" s="46">
@@ -6201,7 +6260,7 @@
       <c r="G231" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H231" s="64"/>
+      <c r="H231" s="63"/>
     </row>
     <row r="232" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B232" s="46" t="s">
@@ -6217,10 +6276,10 @@
         <v>253</v>
       </c>
       <c r="F232" s="33">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G232" s="45"/>
-      <c r="H232" s="67">
+      <c r="H232" s="66">
         <v>45590</v>
       </c>
     </row>
@@ -6251,7 +6310,7 @@
       <c r="D234" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E234" s="61">
+      <c r="E234" s="60">
         <v>15</v>
       </c>
       <c r="F234" s="46">
@@ -6271,7 +6330,7 @@
       <c r="D235" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E235" s="61" t="s">
+      <c r="E235" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F235" s="46">
@@ -6280,7 +6339,7 @@
       <c r="G235" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H235" s="67">
+      <c r="H235" s="66">
         <v>45529</v>
       </c>
     </row>
@@ -6298,9 +6357,9 @@
         <v>253</v>
       </c>
       <c r="F236" s="33">
-        <v>0</v>
-      </c>
-      <c r="H236" s="67">
+        <v>1</v>
+      </c>
+      <c r="H236" s="66">
         <v>45682</v>
       </c>
     </row>
@@ -6314,7 +6373,7 @@
       <c r="D237" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="E237" s="61">
+      <c r="E237" s="60">
         <v>3</v>
       </c>
       <c r="F237" s="46">
@@ -6323,7 +6382,7 @@
       <c r="G237" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H237" s="67"/>
+      <c r="H237" s="66"/>
     </row>
     <row r="238" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238" s="46" t="s">
@@ -6342,7 +6401,7 @@
         <v>2</v>
       </c>
       <c r="G238" s="45"/>
-      <c r="H238" s="67">
+      <c r="H238" s="66">
         <v>45682</v>
       </c>
     </row>
@@ -6362,7 +6421,7 @@
       <c r="F239" s="33">
         <v>7</v>
       </c>
-      <c r="H239" s="64"/>
+      <c r="H239" s="63"/>
     </row>
     <row r="240" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240" s="46" t="s">
@@ -6374,7 +6433,7 @@
       <c r="D240" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E240" s="61">
+      <c r="E240" s="60">
         <v>1</v>
       </c>
       <c r="F240" s="46">
@@ -6398,10 +6457,10 @@
         <v>253</v>
       </c>
       <c r="F241" s="29">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G241" s="17"/>
-      <c r="H241" s="67">
+      <c r="H241" s="66">
         <v>45529</v>
       </c>
     </row>
@@ -6414,17 +6473,17 @@
       </c>
       <c r="F242" s="43">
         <f>SUM(F224:F241)-SUM(F221:F223)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G242" s="17"/>
-      <c r="H242" s="64"/>
+      <c r="H242" s="63"/>
     </row>
     <row r="243" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C243" s="15"/>
       <c r="D243" s="15"/>
       <c r="E243" s="16"/>
       <c r="F243" s="15"/>
-      <c r="H243" s="64"/>
+      <c r="H243" s="63"/>
     </row>
     <row r="244" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G244" s="17"/>
@@ -6479,7 +6538,7 @@
         <v>8</v>
       </c>
       <c r="F248" s="29">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G248" s="50"/>
     </row>
@@ -6555,7 +6614,7 @@
         <v>15</v>
       </c>
       <c r="F254" s="33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G254" s="45"/>
     </row>
@@ -6586,7 +6645,7 @@
       <c r="D256" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="E256" s="61">
+      <c r="E256" s="60">
         <v>1</v>
       </c>
       <c r="F256" s="46">
@@ -6610,9 +6669,9 @@
         <v>253</v>
       </c>
       <c r="F257" s="33">
-        <v>5</v>
-      </c>
-      <c r="H257" s="67">
+        <v>6</v>
+      </c>
+      <c r="H257" s="66">
         <v>45627</v>
       </c>
     </row>
@@ -6620,7 +6679,7 @@
       <c r="B258" s="53"/>
       <c r="C258" s="53"/>
       <c r="D258" s="53"/>
-      <c r="E258" s="60"/>
+      <c r="E258" s="59"/>
       <c r="F258" s="53"/>
     </row>
     <row r="259" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -6637,7 +6696,7 @@
         <v>30</v>
       </c>
       <c r="F259" s="33">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G259" s="45"/>
     </row>
@@ -6651,7 +6710,7 @@
       <c r="D260" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E260" s="61">
+      <c r="E260" s="60">
         <v>9</v>
       </c>
       <c r="F260" s="46">
@@ -6675,9 +6734,9 @@
         <v>253</v>
       </c>
       <c r="F261" s="33">
-        <v>16</v>
-      </c>
-      <c r="H261" s="67">
+        <v>18</v>
+      </c>
+      <c r="H261" s="66">
         <v>45534</v>
       </c>
     </row>
@@ -6691,7 +6750,7 @@
       <c r="D262" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="E262" s="61">
+      <c r="E262" s="60">
         <v>3</v>
       </c>
       <c r="F262" s="46">
@@ -6700,7 +6759,7 @@
       <c r="G262" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H262" s="67"/>
+      <c r="H262" s="66"/>
     </row>
     <row r="263" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B263" s="46" t="s">
@@ -6718,7 +6777,7 @@
       <c r="F263" s="33">
         <v>4</v>
       </c>
-      <c r="H263" s="67">
+      <c r="H263" s="66">
         <v>45627</v>
       </c>
     </row>
@@ -6749,7 +6808,7 @@
       <c r="D265" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E265" s="61">
+      <c r="E265" s="60">
         <v>1</v>
       </c>
       <c r="F265" s="46">
@@ -6776,7 +6835,7 @@
         <v>1</v>
       </c>
       <c r="G266" s="45"/>
-      <c r="H266" s="67">
+      <c r="H266" s="66">
         <v>45310</v>
       </c>
     </row>
@@ -6868,7 +6927,7 @@
         <v>10</v>
       </c>
       <c r="F275" s="29">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G275" s="17"/>
     </row>
@@ -6943,7 +7002,7 @@
         <v>7</v>
       </c>
       <c r="F281" s="33">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G281" s="45"/>
     </row>
@@ -6961,7 +7020,7 @@
         <v>22</v>
       </c>
       <c r="F282" s="33">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="283" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -7004,7 +7063,7 @@
         <v>2</v>
       </c>
       <c r="F285" s="33">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G285" s="45"/>
     </row>
@@ -7018,7 +7077,7 @@
       <c r="D286" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="E286" s="61">
+      <c r="E286" s="60">
         <v>1</v>
       </c>
       <c r="F286" s="46">
@@ -7044,7 +7103,7 @@
       <c r="F287" s="33">
         <v>2</v>
       </c>
-      <c r="H287" s="67">
+      <c r="H287" s="66">
         <v>45515</v>
       </c>
     </row>
@@ -7058,7 +7117,7 @@
       <c r="D288" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E288" s="61">
+      <c r="E288" s="60">
         <v>17</v>
       </c>
       <c r="F288" s="46">
@@ -7067,7 +7126,7 @@
       <c r="G288" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H288" s="67"/>
+      <c r="H288" s="66"/>
     </row>
     <row r="289" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B289" s="46" t="s">
@@ -7083,10 +7142,10 @@
         <v>253</v>
       </c>
       <c r="F289" s="33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G289" s="45"/>
-      <c r="H289" s="67">
+      <c r="H289" s="66">
         <v>45636</v>
       </c>
     </row>
@@ -7100,7 +7159,7 @@
       <c r="D290" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="E290" s="61">
+      <c r="E290" s="60">
         <v>3</v>
       </c>
       <c r="F290" s="46">
@@ -7109,7 +7168,7 @@
       <c r="G290" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="H290" s="67"/>
+      <c r="H290" s="66"/>
     </row>
     <row r="291" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B291" s="46" t="s">
@@ -7128,7 +7187,7 @@
         <v>3</v>
       </c>
       <c r="G291" s="45"/>
-      <c r="H291" s="67">
+      <c r="H291" s="66">
         <v>45636</v>
       </c>
     </row>
@@ -7142,7 +7201,7 @@
       <c r="D292" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="E292" s="61">
+      <c r="E292" s="60">
         <v>3</v>
       </c>
       <c r="F292" s="46">
@@ -7151,7 +7210,7 @@
       <c r="G292" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H292" s="67"/>
+      <c r="H292" s="66"/>
     </row>
     <row r="293" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B293" s="46" t="s">
@@ -7170,7 +7229,7 @@
         <v>3</v>
       </c>
       <c r="G293" s="45"/>
-      <c r="H293" s="67">
+      <c r="H293" s="66">
         <v>45636</v>
       </c>
     </row>
@@ -7199,7 +7258,7 @@
       </c>
       <c r="F296" s="43">
         <f>SUM(F278:F295)-SUM(F275:F277)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G296" s="17"/>
     </row>
@@ -7259,10 +7318,10 @@
       <c r="D302" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="E302" s="62">
-        <v>1</v>
-      </c>
-      <c r="F302" s="63">
+      <c r="E302" s="61">
+        <v>1</v>
+      </c>
+      <c r="F302" s="62">
         <v>7</v>
       </c>
       <c r="G302" s="50" t="s">
@@ -7279,14 +7338,14 @@
       <c r="D303" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E303" s="62" t="s">
+      <c r="E303" s="61" t="s">
         <v>253</v>
       </c>
       <c r="F303" s="49">
         <v>21</v>
       </c>
       <c r="G303" s="50"/>
-      <c r="H303" s="67">
+      <c r="H303" s="66">
         <v>45559</v>
       </c>
     </row>
@@ -7304,10 +7363,10 @@
         <v>253</v>
       </c>
       <c r="F304" s="27">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G304" s="45"/>
-      <c r="H304" s="67">
+      <c r="H304" s="66">
         <v>45657</v>
       </c>
     </row>
@@ -7343,7 +7402,7 @@
         <v>1</v>
       </c>
       <c r="F306" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G306" s="45"/>
     </row>
@@ -7374,7 +7433,7 @@
       <c r="D308" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="E308" s="61">
+      <c r="E308" s="60">
         <v>25</v>
       </c>
       <c r="F308" s="46">
@@ -7398,9 +7457,9 @@
         <v>253</v>
       </c>
       <c r="F309" s="33">
-        <v>5</v>
-      </c>
-      <c r="H309" s="67">
+        <v>6</v>
+      </c>
+      <c r="H309" s="66">
         <v>45564</v>
       </c>
     </row>
@@ -7414,7 +7473,7 @@
       <c r="D310" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="E310" s="60">
+      <c r="E310" s="59">
         <v>16</v>
       </c>
       <c r="F310" s="53">
@@ -7434,7 +7493,7 @@
       <c r="D311" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="E311" s="61" t="s">
+      <c r="E311" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F311" s="46">
@@ -7443,7 +7502,7 @@
       <c r="G311" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H311" s="67">
+      <c r="H311" s="66">
         <v>45518</v>
       </c>
     </row>
@@ -7463,7 +7522,7 @@
       <c r="F312" s="33">
         <v>4</v>
       </c>
-      <c r="H312" s="67">
+      <c r="H312" s="66">
         <v>45532</v>
       </c>
     </row>
@@ -7477,7 +7536,7 @@
       <c r="D313" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="E313" s="61">
+      <c r="E313" s="60">
         <v>15</v>
       </c>
       <c r="F313" s="46">
@@ -7501,9 +7560,9 @@
         <v>253</v>
       </c>
       <c r="F314" s="33">
-        <v>6</v>
-      </c>
-      <c r="H314" s="67">
+        <v>7</v>
+      </c>
+      <c r="H314" s="66">
         <v>45557</v>
       </c>
     </row>
@@ -7521,7 +7580,7 @@
         <v>15</v>
       </c>
       <c r="F315" s="33">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G315" s="45"/>
     </row>
@@ -7535,7 +7594,7 @@
       <c r="D316" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="E316" s="61">
+      <c r="E316" s="60">
         <v>7</v>
       </c>
       <c r="F316" s="46">
@@ -7561,7 +7620,7 @@
       <c r="F317" s="33">
         <v>3</v>
       </c>
-      <c r="H317" s="67">
+      <c r="H317" s="66">
         <v>45550</v>
       </c>
     </row>
@@ -7575,7 +7634,7 @@
       <c r="D318" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E318" s="61">
+      <c r="E318" s="60">
         <v>1</v>
       </c>
       <c r="F318" s="46">
@@ -7595,7 +7654,7 @@
       <c r="D319" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="E319" s="61" t="s">
+      <c r="E319" s="60" t="s">
         <v>253</v>
       </c>
       <c r="F319" s="46">
@@ -7604,7 +7663,7 @@
       <c r="G319" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H319" s="67">
+      <c r="H319" s="66">
         <v>45518</v>
       </c>
     </row>
@@ -7622,9 +7681,9 @@
         <v>253</v>
       </c>
       <c r="F320" s="33">
-        <v>3</v>
-      </c>
-      <c r="H320" s="67">
+        <v>4</v>
+      </c>
+      <c r="H320" s="66">
         <v>45528</v>
       </c>
     </row>
@@ -7638,7 +7697,7 @@
       <c r="D321" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="E321" s="61">
+      <c r="E321" s="60">
         <v>1</v>
       </c>
       <c r="F321" s="46">
@@ -7666,7 +7725,7 @@
         <v>3</v>
       </c>
       <c r="G322" s="17"/>
-      <c r="H322" s="67">
+      <c r="H322" s="66">
         <v>45515</v>
       </c>
     </row>
@@ -7679,7 +7738,7 @@
       </c>
       <c r="F323" s="43">
         <f>SUM(F305:F322)-SUM(F302:F304)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G323" s="17"/>
     </row>
@@ -7733,10 +7792,10 @@
       <c r="D329" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="E329" s="62">
-        <v>1</v>
-      </c>
-      <c r="F329" s="63">
+      <c r="E329" s="61">
+        <v>1</v>
+      </c>
+      <c r="F329" s="62">
         <v>9</v>
       </c>
       <c r="G329" s="45" t="s">
@@ -7753,7 +7812,7 @@
       <c r="D330" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="E330" s="62" t="s">
+      <c r="E330" s="61" t="s">
         <v>253</v>
       </c>
       <c r="F330" s="49">
@@ -7762,7 +7821,7 @@
       <c r="G330" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="H330" s="67">
+      <c r="H330" s="66">
         <v>45537</v>
       </c>
     </row>
@@ -7780,10 +7839,10 @@
         <v>253</v>
       </c>
       <c r="F331" s="27">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G331" s="45"/>
-      <c r="H331" s="67">
+      <c r="H331" s="66">
         <v>45642</v>
       </c>
     </row>
@@ -7826,7 +7885,7 @@
         <v>4</v>
       </c>
       <c r="F334" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G334" s="45"/>
     </row>
@@ -7848,7 +7907,7 @@
       <c r="D336" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="E336" s="61">
+      <c r="E336" s="60">
         <v>15</v>
       </c>
       <c r="F336" s="46">
@@ -7872,10 +7931,10 @@
         <v>253</v>
       </c>
       <c r="F337" s="33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G337" s="45"/>
-      <c r="H337" s="67">
+      <c r="H337" s="66">
         <v>45662</v>
       </c>
     </row>
@@ -7893,7 +7952,7 @@
         <v>47</v>
       </c>
       <c r="F338" s="33">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="339" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -7910,7 +7969,7 @@
         <v>2</v>
       </c>
       <c r="F339" s="33">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="340" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -7930,7 +7989,7 @@
       <c r="D341" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="E341" s="61">
+      <c r="E341" s="60">
         <v>6</v>
       </c>
       <c r="F341" s="46">
@@ -7954,9 +8013,9 @@
         <v>253</v>
       </c>
       <c r="F342" s="33">
-        <v>2</v>
-      </c>
-      <c r="H342" s="67">
+        <v>5</v>
+      </c>
+      <c r="H342" s="66">
         <v>45662</v>
       </c>
     </row>
@@ -7974,7 +8033,7 @@
         <v>3</v>
       </c>
       <c r="F343" s="33">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G343" s="45"/>
     </row>
@@ -7988,7 +8047,7 @@
       <c r="D344" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="E344" s="61">
+      <c r="E344" s="60">
         <v>1</v>
       </c>
       <c r="F344" s="46">
@@ -8015,7 +8074,7 @@
         <v>1</v>
       </c>
       <c r="G345" s="45"/>
-      <c r="H345" s="67">
+      <c r="H345" s="66">
         <v>45662</v>
       </c>
     </row>
@@ -8033,7 +8092,7 @@
         <v>2</v>
       </c>
       <c r="F346" s="33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G346" s="45"/>
     </row>
@@ -8047,7 +8106,7 @@
       <c r="D347" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="E347" s="61">
+      <c r="E347" s="60">
         <v>1</v>
       </c>
       <c r="F347" s="46">
@@ -8071,9 +8130,9 @@
         <v>253</v>
       </c>
       <c r="F348" s="33">
-        <v>0</v>
-      </c>
-      <c r="H348" s="67">
+        <v>1</v>
+      </c>
+      <c r="H348" s="66">
         <v>45662</v>
       </c>
     </row>
@@ -8093,7 +8152,7 @@
       </c>
       <c r="F350" s="43">
         <f>SUM(F332:F349)-SUM(F329:F331)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="351" spans="2:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -8122,7 +8181,7 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8208,13 +8267,13 @@
         <v>21</v>
       </c>
       <c r="E7" s="30">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F7" s="31">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G7" s="32">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K7" s="51"/>
     </row>
@@ -8229,13 +8288,13 @@
         <v>41</v>
       </c>
       <c r="E8" s="30">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F8" s="31">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="G8" s="32">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8243,19 +8302,19 @@
         <v>3</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E9" s="30">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="31">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="G9" s="32">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8263,19 +8322,19 @@
         <v>4</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E10" s="30">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="31">
         <v>87</v>
       </c>
       <c r="G10" s="32">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -8283,19 +8342,19 @@
         <v>5</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E11" s="30">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F11" s="31">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="32">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8309,13 +8368,13 @@
         <v>44</v>
       </c>
       <c r="E12" s="30">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F12" s="31">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="G12" s="32">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8329,13 +8388,13 @@
         <v>17</v>
       </c>
       <c r="E13" s="30">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F13" s="31">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G13" s="32">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8349,13 +8408,13 @@
         <v>234</v>
       </c>
       <c r="E14" s="30">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F14" s="31">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="G14" s="32">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8369,13 +8428,13 @@
         <v>251</v>
       </c>
       <c r="E15" s="30">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F15" s="31">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G15" s="32">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8383,19 +8442,19 @@
         <v>10</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E16" s="30">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F16" s="31">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G16" s="32">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -8403,19 +8462,19 @@
         <v>11</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E17" s="30">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" s="31">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G17" s="32">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -8423,19 +8482,19 @@
         <v>12</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E18" s="30">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F18" s="31">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G18" s="32">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -8443,19 +8502,19 @@
         <v>13</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E19" s="30">
         <v>3</v>
       </c>
       <c r="F19" s="31">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G19" s="32">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -8590,33 +8649,45 @@
       <c r="B10" s="50"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>348</v>
+      </c>
       <c r="D11" s="45" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="57"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C12" s="57" t="s">
+        <v>348</v>
+      </c>
       <c r="D12" s="45" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
+      <c r="B13" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>348</v>
+      </c>
       <c r="D13" s="45" t="s">
         <v>44</v>
       </c>
@@ -8626,9 +8697,13 @@
       <c r="A14" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="45" t="s">
+      <c r="B14" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>361</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>234</v>
       </c>
       <c r="F14" s="57"/>
@@ -8646,13 +8721,33 @@
       <c r="B16" s="50"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+      <c r="A17" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>352</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>251</v>
+      </c>
       <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="A18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>365</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>364</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>21</v>
+      </c>
       <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -8669,8 +8764,14 @@
       <c r="F20" s="57"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="45" t="s">
+        <v>234</v>
+      </c>
       <c r="B21" s="57"/>
       <c r="C21" s="57"/>
+      <c r="D21" s="45" t="s">
+        <v>17</v>
+      </c>
       <c r="F21" s="57"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>